<commit_message>
Completing first 18 roles
</commit_message>
<xml_diff>
--- a/githubaction_roles.xlsx
+++ b/githubaction_roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudelligentcom-my.sharepoint.com/personal/ameera_haider_cloudelligent_com/Documents/Desktop/Cellanome/IAM-Roles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_3EA5FB139134EF62A5A0D6F0505ED87656CDFAB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A4CD154-1549-4ABB-95FF-3BBBED69CED4}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_3EA5FB139134EF62A5A0D6F0505ED87656CDFAB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D76C063D-10A4-4BAC-B7EB-61289C6F2021}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="960" windowWidth="21348" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>RoleName</t>
   </si>
@@ -215,6 +215,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,7 +509,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,83 +643,95 @@
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>